<commit_message>
Revert "Update 몬스터 기획서.xlsx"
This reverts commit 9671077d36d66231425bf6e72dfffda191e8aa00.
</commit_message>
<xml_diff>
--- a/Design/몬스터 기획서.xlsx
+++ b/Design/몬스터 기획서.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\바탕 화면\plum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42E848A-0BF3-40B0-A87A-A1C0EFBC0F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A14FFA1-D65B-4CF1-AB15-D0DB2BEB043F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{6ED0029A-6F1E-4A92-AB37-7B6700187FC9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{6ED0029A-6F1E-4A92-AB37-7B6700187FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="몬스터 기획서" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="466">
   <si>
     <t>version</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -934,10 +934,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>속성 : 무(15%), 흙(35%), 전기(25%), 불(25%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>특성 : 거대한, 단단한</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>속성 : 전기(40%), 불(30%), 흙(20%), 물(10%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>7.2 기믹</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1834,32 +1842,6 @@
   <si>
     <t>적용가능한 몬스터 분류</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>무속성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>불속성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>흙속성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물속성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>전기속성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>속성 : 흙(35%), 전기(25%), 불(25%), 무(15%)</t>
-  </si>
-  <si>
-    <t>속성 : 전기(40%), 불(30%), 흙(20%), 물(10%)</t>
   </si>
 </sst>
 </file>
@@ -3052,1835 +3034,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>525780</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>51716</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="그림 2" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE4BDB00-61F0-49D5-AE9E-236380A4AE12}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="72289" t="12787" r="3213" b="55245"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5219700" y="1028700"/>
-          <a:ext cx="1028700" cy="1011836"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>90940</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="그림 3" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D748C21A-91B5-4464-B57F-C1DA681024A6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="9237" t="61805" r="69880" b="5695"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6583680" y="1028700"/>
-          <a:ext cx="883420" cy="1036320"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>144779</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>96288</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61304739-50EC-4F2F-987B-B6812DA3BD9A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="29719" t="63402" r="43775" b="4097"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7848600" y="1028699"/>
-          <a:ext cx="1143000" cy="1056409"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>205739</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>13694</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="그림 12" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5C462BB-D89F-49C3-B4AA-353B8166BE5D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="15232" t="55440" r="55867" b="4663"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5836920" y="3078479"/>
-          <a:ext cx="1089660" cy="1133835"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>213359</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>26510</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="그림 13" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20F112A6-7A72-4867-9375-C2AC9740D7B0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="72252" t="24353" b="29016"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7277100" y="3086099"/>
-          <a:ext cx="899160" cy="1139031"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>220979</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19472</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="그림 14" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF494F54-9F66-456A-9567-C534353E0BC8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="27729" r="54696" b="58549"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8724900" y="3093719"/>
-          <a:ext cx="632460" cy="1124373"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>19792</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="그림 15" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09F346D7-8E0F-44C5-A15B-8F64A44216BD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="3905" t="25389" r="66022" b="31606"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9799320" y="3101340"/>
-          <a:ext cx="1036320" cy="1117072"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>5079</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>662940</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>182478</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="그림 16" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7AFFAC8-AD12-40F8-AE86-3C899D482C90}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="26046" t="53926" r="51459"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5867400" y="5087619"/>
-          <a:ext cx="830580" cy="1282299"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>55296</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>182880</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="그림 17" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD0AD1F0-4F0A-4500-9E9B-0CCE814A4481}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="51304" t="59162" r="26202" b="2094"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7086600" y="5052060"/>
-          <a:ext cx="1015416" cy="1318260"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>205740</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="그림 18" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF764CEF-BA90-41B9-BC98-3C1DEFE50CC0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="41438" t="1047" r="40010" b="63875"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8473440" y="5013960"/>
-          <a:ext cx="967740" cy="1379220"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>182879</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>205434</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="그림 19" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94C12A86-BF67-41EB-8F40-72FCE9571E84}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="76955" t="23561" r="3312" b="35077"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9966960" y="5044439"/>
-          <a:ext cx="853440" cy="1348435"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>457199</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>655422</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="그림 20" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2339E8EF-8D71-4989-B835-F02A67BAD93C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="26604" t="60427" r="49615" b="1"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5821679" y="7124700"/>
-          <a:ext cx="868783" cy="1089660"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>45719</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>655320</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>132414</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="그림 21" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09D30B3D-9C50-47CE-B541-30E7DE549B14}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="49982" t="61497" r="28654" b="-1069"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7178040" y="7117079"/>
-          <a:ext cx="853440" cy="1191595"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>100864</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="23" name="그림 22" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDFACC43-562A-4D89-9579-425754E06111}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="84245" t="42246" r="438" b="34759"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8519160" y="7147559"/>
-          <a:ext cx="998220" cy="1129565"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>631237</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="그림 23" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48F9F141-EE4D-4DBF-8DF0-243B34F37363}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="74571" t="56684" r="6484"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9982200" y="7101840"/>
-          <a:ext cx="707437" cy="1219200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>263492</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="그림 24" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF5D87F-56E7-4855-9E24-784D449E221D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="1186" t="24122" r="66798" b="45989"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6210300" y="9052560"/>
-          <a:ext cx="1429352" cy="1005840"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>99060</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>144378</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="그림 27" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B51381B-9435-4CF0-9C12-1A73F418A44C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="54150" t="53486" r="23320" b="15051"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7810500" y="9029699"/>
-          <a:ext cx="1005840" cy="1058779"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>37536</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="29" name="그림 28" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D465183E-2932-4640-8B60-C094F0C21360}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="3558" t="47717" r="75889" b="23966"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9090660" y="9052560"/>
-          <a:ext cx="1005276" cy="1043940"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="그림 29" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68CFF9BA-FB91-4E7F-AB73-0871D64BFFAC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="75099" t="48243" r="1186" b="21868"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="10439400" y="9083040"/>
-          <a:ext cx="1066800" cy="1013460"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>3420</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="31" name="그림 30" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0286A877-B390-48A0-B717-64CE9C21C23C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="55814" t="7713" r="13954" b="49607"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6507480" y="11056619"/>
-          <a:ext cx="1242060" cy="1321681"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>301200</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="그림 32" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9297F143-05C9-4D18-93DC-391E09191A7D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="8527" t="44222" r="52326" b="243"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8427719" y="11018519"/>
-          <a:ext cx="1261321" cy="1348741"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>205739</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>38455</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="그림 33" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D5914EC-25BF-437C-AD54-A6D02A0E5E66}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="13307" t="10476" r="53994" b="44124"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4983480" y="11033759"/>
-          <a:ext cx="1318260" cy="1379576"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>152094</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="그림 34" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50BF789C-0FF2-4D71-80D9-5CA5FD28550F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="-1165" t="38659" r="72024" b="28351"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="11529060" y="13007339"/>
-          <a:ext cx="1508760" cy="1287475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>220979</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>249187</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="그림 35" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C5DD9EF-D216-45FB-B8B3-EAF42BDCC875}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="6994" t="10825" r="65808" b="54639"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5585459" y="12992100"/>
-          <a:ext cx="1369328" cy="1310640"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>393154</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="그림 36" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{442C477C-711C-41F3-8365-2104AFE9C651}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="12822" t="59279" r="48324"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7528559" y="13060680"/>
-          <a:ext cx="1581875" cy="1249680"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>7619</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>162592</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="그림 37" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEAD45C3-DA9B-42A5-ACF4-915E5355FA62}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="75377" t="36598" b="31443"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9662160" y="13045439"/>
-          <a:ext cx="1287780" cy="1259873"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>24139</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="그림 38" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E22E3BD-12FF-4194-B936-97EB62C5ACD6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="50575" t="55913" r="22988" b="-2033"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5897880" y="15194280"/>
-          <a:ext cx="899160" cy="1182379"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>502919</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>198119</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>43486</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="40" name="그림 39" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{595E6CC4-81CA-4DE2-B719-0C43BC739523}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="69732" t="33040" b="16639"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7208519" y="15224759"/>
-          <a:ext cx="881687" cy="1104901"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>502920</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>617220</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>193638</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="그림 40" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31C04216-EAAB-4747-8DC1-1AFDCCAFE750}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect t="38631" r="73946" b="12572"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="8549640" y="15217139"/>
-          <a:ext cx="784860" cy="1108039"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>36884</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>198120</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="그림 42" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA850E1C-FD40-43B5-891F-0F9FE935233A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="4981" t="14232" r="72414" b="50695"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9814560" y="15217139"/>
-          <a:ext cx="951284" cy="1112521"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>213360</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="44" name="그림 43" descr="screenshot">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8DA0478-0781-43F1-8E8D-25B2AE2B3ED3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="25296" t="58206" r="54150" b="5612"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="11986260" y="9052560"/>
-          <a:ext cx="792480" cy="1051560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5194,7 +3347,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="44" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -5233,7 +3386,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -5252,7 +3405,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="44"/>
@@ -5286,7 +3439,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C6" s="44"/>
       <c r="D6" s="44"/>
@@ -5317,7 +3470,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="41" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -5334,32 +3487,32 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -5381,7 +3534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE54A3D-9C9F-418C-AD1A-92217D66A9D7}">
   <dimension ref="A1:AE162"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A105" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
@@ -5389,87 +3542,87 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" s="42" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" s="15" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" s="15" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="15" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="15" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="42" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" s="42" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.4">
@@ -5490,7 +3643,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" s="43" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.4">
@@ -5647,17 +3800,17 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A36" s="15" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.4">
@@ -5829,12 +3982,12 @@
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A51" s="15" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.4">
@@ -5844,12 +3997,12 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A57" s="45" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B57" s="45"/>
       <c r="C57" s="21" t="s">
@@ -6118,7 +4271,7 @@
       <c r="E66" s="20"/>
       <c r="F66" s="20"/>
       <c r="G66" s="22" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.4">
@@ -6128,12 +4281,12 @@
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A70" s="45" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B70" s="45"/>
       <c r="C70" s="21" t="s">
@@ -6490,7 +4643,7 @@
         <v>56</v>
       </c>
       <c r="H79" s="48" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="I79" s="49"/>
       <c r="J79" s="49"/>
@@ -6531,7 +4684,7 @@
         <v>55</v>
       </c>
       <c r="H80" s="48" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="I80" s="49"/>
       <c r="J80" s="49"/>
@@ -6568,7 +4721,7 @@
         <v>10</v>
       </c>
       <c r="G81" s="13" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.4">
@@ -6579,7 +4732,7 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A83" s="38"/>
       <c r="B83" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>64</v>
@@ -6587,21 +4740,21 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.4">
       <c r="G84" s="13" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A85" s="39"/>
       <c r="B85" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.4">
       <c r="G86" s="13" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.4">
@@ -6609,7 +4762,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A89" s="15" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.4">
@@ -6737,12 +4890,12 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A102" s="15" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.4">
@@ -6753,7 +4906,7 @@
         <v>77</v>
       </c>
       <c r="D106" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.4">
@@ -6875,12 +5028,12 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A115" s="15" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.4">
@@ -6926,12 +5079,12 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.4">
@@ -6946,34 +5099,34 @@
     </row>
     <row r="131" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="132" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A132" s="51" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B132" s="51"/>
       <c r="C132" s="51"/>
       <c r="D132" s="30" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E132" s="51" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F132" s="51"/>
       <c r="G132" s="30" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H132" s="47" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I132" s="47"/>
       <c r="J132" s="30" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="K132" s="47" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="L132" s="47"/>
       <c r="M132" s="47"/>
@@ -6983,7 +5136,7 @@
       <c r="Q132" s="47"/>
       <c r="R132" s="47"/>
       <c r="S132" s="47" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="T132" s="47"/>
       <c r="U132" s="47"/>
@@ -6992,7 +5145,7 @@
     </row>
     <row r="133" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A133" s="52" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B133" s="52"/>
       <c r="C133" s="52"/>
@@ -7000,7 +5153,7 @@
         <v>10</v>
       </c>
       <c r="E133" s="52" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F133" s="52"/>
       <c r="G133" s="29">
@@ -7012,7 +5165,7 @@
         <v>10</v>
       </c>
       <c r="K133" s="45" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="L133" s="45"/>
       <c r="M133" s="45"/>
@@ -7022,7 +5175,7 @@
       <c r="Q133" s="45"/>
       <c r="R133" s="45"/>
       <c r="S133" s="45" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="T133" s="45"/>
       <c r="U133" s="45"/>
@@ -7035,7 +5188,7 @@
       <c r="C134" s="45"/>
       <c r="D134" s="45"/>
       <c r="E134" s="52" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F134" s="52"/>
       <c r="G134" s="29">
@@ -7047,7 +5200,7 @@
         <v>10</v>
       </c>
       <c r="K134" s="45" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="L134" s="45"/>
       <c r="M134" s="45"/>
@@ -7068,7 +5221,7 @@
       <c r="C135" s="45"/>
       <c r="D135" s="45"/>
       <c r="E135" s="29" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F135" s="29"/>
       <c r="G135" s="29">
@@ -7080,7 +5233,7 @@
         <v>10</v>
       </c>
       <c r="K135" s="45" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="L135" s="45"/>
       <c r="M135" s="45"/>
@@ -7101,7 +5254,7 @@
       <c r="C136" s="45"/>
       <c r="D136" s="45"/>
       <c r="E136" s="28" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F136" s="28"/>
       <c r="G136" s="29">
@@ -7113,7 +5266,7 @@
         <v>10</v>
       </c>
       <c r="K136" s="46" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="L136" s="46"/>
       <c r="M136" s="46"/>
@@ -7134,7 +5287,7 @@
       <c r="C137" s="45"/>
       <c r="D137" s="45"/>
       <c r="E137" s="28" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F137" s="28"/>
       <c r="G137" s="29">
@@ -7146,7 +5299,7 @@
         <v>10</v>
       </c>
       <c r="K137" s="46" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="L137" s="46"/>
       <c r="M137" s="46"/>
@@ -7156,7 +5309,7 @@
       <c r="Q137" s="46"/>
       <c r="R137" s="46"/>
       <c r="S137" s="45" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="T137" s="45"/>
       <c r="U137" s="45"/>
@@ -7169,7 +5322,7 @@
       <c r="C138" s="45"/>
       <c r="D138" s="45"/>
       <c r="E138" s="28" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F138" s="28"/>
       <c r="G138" s="29">
@@ -7181,7 +5334,7 @@
         <v>10</v>
       </c>
       <c r="K138" s="46" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="L138" s="46"/>
       <c r="M138" s="46"/>
@@ -7198,7 +5351,7 @@
     </row>
     <row r="139" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A139" s="52" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B139" s="52"/>
       <c r="C139" s="52"/>
@@ -7206,21 +5359,21 @@
         <v>20</v>
       </c>
       <c r="E139" s="28" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F139" s="28"/>
       <c r="G139" s="29">
         <v>11</v>
       </c>
       <c r="H139" s="45" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I139" s="45"/>
       <c r="J139" s="29">
         <v>11</v>
       </c>
       <c r="K139" s="45" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="L139" s="45"/>
       <c r="M139" s="45"/>
@@ -7230,7 +5383,7 @@
       <c r="Q139" s="45"/>
       <c r="R139" s="45"/>
       <c r="S139" s="45" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="T139" s="45"/>
       <c r="U139" s="45"/>
@@ -7246,14 +5399,14 @@
       <c r="F140" s="45"/>
       <c r="G140" s="29"/>
       <c r="H140" s="45" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I140" s="45"/>
       <c r="J140" s="29">
         <v>21</v>
       </c>
       <c r="K140" s="45" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="L140" s="45"/>
       <c r="M140" s="45"/>
@@ -7277,14 +5430,14 @@
       <c r="F141" s="45"/>
       <c r="G141" s="29"/>
       <c r="H141" s="45" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I141" s="45"/>
       <c r="J141" s="29">
         <v>31</v>
       </c>
       <c r="K141" s="45" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="L141" s="45"/>
       <c r="M141" s="45"/>
@@ -7308,14 +5461,14 @@
       <c r="F142" s="45"/>
       <c r="G142" s="29"/>
       <c r="H142" s="46" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="I142" s="46"/>
       <c r="J142" s="29">
         <v>41</v>
       </c>
       <c r="K142" s="45" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="L142" s="45"/>
       <c r="M142" s="45"/>
@@ -7336,21 +5489,21 @@
       <c r="C143" s="45"/>
       <c r="D143" s="45"/>
       <c r="E143" s="28" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F143" s="28"/>
       <c r="G143" s="29">
         <v>21</v>
       </c>
       <c r="H143" s="45" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I143" s="45"/>
       <c r="J143" s="29">
         <v>11</v>
       </c>
       <c r="K143" s="45" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="L143" s="45"/>
       <c r="M143" s="45"/>
@@ -7374,14 +5527,14 @@
       <c r="F144" s="45"/>
       <c r="G144" s="29"/>
       <c r="H144" s="45" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I144" s="45"/>
       <c r="J144" s="29">
         <v>21</v>
       </c>
       <c r="K144" s="45" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="L144" s="45"/>
       <c r="M144" s="45"/>
@@ -7405,14 +5558,14 @@
       <c r="F145" s="45"/>
       <c r="G145" s="29"/>
       <c r="H145" s="45" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I145" s="45"/>
       <c r="J145" s="29">
         <v>31</v>
       </c>
       <c r="K145" s="45" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="L145" s="45"/>
       <c r="M145" s="45"/>
@@ -7436,14 +5589,14 @@
       <c r="F146" s="45"/>
       <c r="G146" s="29"/>
       <c r="H146" s="46" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I146" s="46"/>
       <c r="J146" s="29">
         <v>41</v>
       </c>
       <c r="K146" s="45" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="L146" s="45"/>
       <c r="M146" s="45"/>
@@ -7464,21 +5617,21 @@
       <c r="C147" s="45"/>
       <c r="D147" s="45"/>
       <c r="E147" s="28" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F147" s="28"/>
       <c r="G147" s="29">
         <v>31</v>
       </c>
       <c r="H147" s="45" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I147" s="45"/>
       <c r="J147" s="29">
         <v>11</v>
       </c>
       <c r="K147" s="45" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="L147" s="45"/>
       <c r="M147" s="45"/>
@@ -7488,7 +5641,7 @@
       <c r="Q147" s="45"/>
       <c r="R147" s="45"/>
       <c r="S147" s="45" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="T147" s="45"/>
       <c r="U147" s="45"/>
@@ -7504,14 +5657,14 @@
       <c r="F148" s="45"/>
       <c r="G148" s="29"/>
       <c r="H148" s="45" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I148" s="45"/>
       <c r="J148" s="29">
         <v>21</v>
       </c>
       <c r="K148" s="45" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="L148" s="45"/>
       <c r="M148" s="45"/>
@@ -7535,14 +5688,14 @@
       <c r="F149" s="45"/>
       <c r="G149" s="29"/>
       <c r="H149" s="45" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I149" s="45"/>
       <c r="J149" s="29">
         <v>31</v>
       </c>
       <c r="K149" s="45" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="L149" s="45"/>
       <c r="M149" s="45"/>
@@ -7566,14 +5719,14 @@
       <c r="F150" s="45"/>
       <c r="G150" s="29"/>
       <c r="H150" s="46" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I150" s="46"/>
       <c r="J150" s="29">
         <v>41</v>
       </c>
       <c r="K150" s="45" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="L150" s="45"/>
       <c r="M150" s="45"/>
@@ -7594,21 +5747,21 @@
       <c r="C151" s="45"/>
       <c r="D151" s="45"/>
       <c r="E151" s="28" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F151" s="28"/>
       <c r="G151" s="29">
         <v>41</v>
       </c>
       <c r="H151" s="45" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I151" s="45"/>
       <c r="J151" s="29">
         <v>11</v>
       </c>
       <c r="K151" s="45" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="L151" s="45"/>
       <c r="M151" s="45"/>
@@ -7632,14 +5785,14 @@
       <c r="F152" s="46"/>
       <c r="G152" s="29"/>
       <c r="H152" s="45" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I152" s="45"/>
       <c r="J152" s="29">
         <v>21</v>
       </c>
       <c r="K152" s="45" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="L152" s="45"/>
       <c r="M152" s="45"/>
@@ -7663,14 +5816,14 @@
       <c r="F153" s="46"/>
       <c r="G153" s="29"/>
       <c r="H153" s="45" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I153" s="45"/>
       <c r="J153" s="29">
         <v>31</v>
       </c>
       <c r="K153" s="45" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="L153" s="45"/>
       <c r="M153" s="45"/>
@@ -7694,14 +5847,14 @@
       <c r="F154" s="46"/>
       <c r="G154" s="29"/>
       <c r="H154" s="46" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I154" s="46"/>
       <c r="J154" s="29">
         <v>41</v>
       </c>
       <c r="K154" s="45" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="L154" s="45"/>
       <c r="M154" s="45"/>
@@ -7718,7 +5871,7 @@
     </row>
     <row r="155" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A155" s="52" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B155" s="52"/>
       <c r="C155" s="52"/>
@@ -7731,14 +5884,14 @@
         <v>10</v>
       </c>
       <c r="H155" s="45" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="I155" s="45"/>
       <c r="J155" s="29">
         <v>11</v>
       </c>
       <c r="K155" s="45" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L155" s="45"/>
       <c r="M155" s="45"/>
@@ -7762,14 +5915,14 @@
       <c r="F156" s="45"/>
       <c r="G156" s="29"/>
       <c r="H156" s="46" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="I156" s="46"/>
       <c r="J156" s="28">
         <v>21</v>
       </c>
       <c r="K156" s="45" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="L156" s="45"/>
       <c r="M156" s="45"/>
@@ -7793,14 +5946,14 @@
       <c r="F157" s="45"/>
       <c r="G157" s="29"/>
       <c r="H157" s="46" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="I157" s="46"/>
       <c r="J157" s="28">
         <v>31</v>
       </c>
       <c r="K157" s="45" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="L157" s="45"/>
       <c r="M157" s="45"/>
@@ -7824,14 +5977,14 @@
       <c r="F158" s="45"/>
       <c r="G158" s="29"/>
       <c r="H158" s="46" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="I158" s="46"/>
       <c r="J158" s="28">
         <v>41</v>
       </c>
       <c r="K158" s="45" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="L158" s="45"/>
       <c r="M158" s="45"/>
@@ -7855,14 +6008,14 @@
       <c r="F159" s="45"/>
       <c r="G159" s="29"/>
       <c r="H159" s="46" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="I159" s="46"/>
       <c r="J159" s="28">
         <v>51</v>
       </c>
       <c r="K159" s="45" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="L159" s="45"/>
       <c r="M159" s="45"/>
@@ -7886,14 +6039,14 @@
       <c r="F160" s="45"/>
       <c r="G160" s="29"/>
       <c r="H160" s="46" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="I160" s="46"/>
       <c r="J160" s="28">
         <v>61</v>
       </c>
       <c r="K160" s="45" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="L160" s="45"/>
       <c r="M160" s="45"/>
@@ -7910,7 +6063,7 @@
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -8123,301 +6276,192 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0229D3AE-EA7B-4ECD-8B36-2AF685B19998}">
-  <dimension ref="B1:S79"/>
+  <dimension ref="B1:E79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B2" s="26" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E7" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E9" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="I11" t="s">
-        <v>464</v>
-      </c>
-      <c r="K11" t="s">
-        <v>465</v>
-      </c>
-      <c r="M11" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E17" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E19" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="J21" t="s">
-        <v>464</v>
-      </c>
-      <c r="L21" t="s">
-        <v>467</v>
-      </c>
-      <c r="N21" t="s">
-        <v>465</v>
-      </c>
-      <c r="P21" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B23" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E26" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E28" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="J30" t="s">
-        <v>464</v>
-      </c>
-      <c r="L30" t="s">
-        <v>466</v>
-      </c>
-      <c r="N30" t="s">
-        <v>467</v>
-      </c>
-      <c r="P30" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B32" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E33" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E35" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.4">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E37" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="J39" t="s">
-        <v>464</v>
-      </c>
-      <c r="L39" t="s">
-        <v>467</v>
-      </c>
-      <c r="N39" t="s">
-        <v>468</v>
-      </c>
-      <c r="P39" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B41" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E42" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E44" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.4">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E46" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="K47" t="s">
-        <v>464</v>
-      </c>
-      <c r="M47" t="s">
-        <v>467</v>
-      </c>
-      <c r="O47" t="s">
-        <v>466</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>465</v>
-      </c>
-      <c r="S47" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B50" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E51" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E53" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E55" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="I57" t="s">
-        <v>467</v>
-      </c>
-      <c r="K57" t="s">
-        <v>464</v>
-      </c>
-      <c r="N57" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B59" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E60" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E62" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.4">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E64" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="66" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="J66" t="s">
-        <v>466</v>
-      </c>
-      <c r="M66" t="s">
-        <v>468</v>
-      </c>
-      <c r="P66" t="s">
-        <v>465</v>
-      </c>
-      <c r="S66" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="68" spans="2:19" x14ac:dyDescent="0.4">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E69" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="71" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E71" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="73" spans="2:19" x14ac:dyDescent="0.4">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.4">
       <c r="E73" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="75" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="J75" t="s">
-        <v>468</v>
-      </c>
-      <c r="L75" t="s">
-        <v>465</v>
-      </c>
-      <c r="N75" t="s">
-        <v>466</v>
-      </c>
-      <c r="P75" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="77" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="79" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B79" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -8434,50 +6478,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596D889C-6BC7-4AA6-B2AE-A17E32433E8E}">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.4">
@@ -8497,12 +6541,12 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
@@ -8557,7 +6601,7 @@
         <v>153</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
@@ -8571,7 +6615,7 @@
         <v>154</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
@@ -8687,7 +6731,7 @@
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
       <c r="F37" s="45" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="G37" s="45"/>
       <c r="H37" s="45"/>
@@ -8706,7 +6750,7 @@
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
       <c r="F38" s="45" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="G38" s="45"/>
       <c r="H38" s="45"/>
@@ -8725,7 +6769,7 @@
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
       <c r="F39" s="45" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="G39" s="45"/>
       <c r="H39" s="45"/>
@@ -8744,7 +6788,7 @@
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
       <c r="F40" s="45" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G40" s="45"/>
       <c r="H40" s="45"/>
@@ -8785,7 +6829,7 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B43" s="13" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="25"/>
@@ -8902,25 +6946,25 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A58" s="15" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.4">
       <c r="B64" s="31" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C64" s="45" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D64" s="45"/>
       <c r="E64" s="45"/>
@@ -8933,10 +6977,10 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B65" s="31" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C65" s="45" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D65" s="45"/>
       <c r="E65" s="45"/>
@@ -8949,30 +6993,30 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B66" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A68" s="15" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B73" s="34" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C73" s="45" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="D73" s="45"/>
       <c r="E73" s="45"/>
@@ -8986,10 +7030,10 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B74" s="34" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C74" s="45" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D74" s="45"/>
       <c r="E74" s="45"/>
@@ -9003,10 +7047,10 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B75" s="34" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C75" s="45" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D75" s="45"/>
       <c r="E75" s="45"/>
@@ -9060,7 +7104,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -9077,7 +7121,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -9090,59 +7134,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF28440-5CF1-47B7-8D33-8E6B67D19736}">
   <dimension ref="B1:N126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74:L125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.4">
       <c r="D1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="F1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B2" s="29" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>146</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>345</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>347</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>352</v>
+      </c>
+      <c r="H2" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>348</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>345</v>
-      </c>
-      <c r="G2" s="29" t="s">
-        <v>350</v>
-      </c>
-      <c r="H2" s="29" t="s">
-        <v>341</v>
-      </c>
       <c r="I2" s="29" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="M2" s="29" t="s">
         <v>204</v>
@@ -9159,31 +7203,31 @@
         <v>10</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="M3" s="29" t="s">
         <v>206</v>
@@ -9206,7 +7250,7 @@
         <v>100</v>
       </c>
       <c r="F4" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G4" s="29">
         <v>10</v>
@@ -9247,7 +7291,7 @@
         <v>100</v>
       </c>
       <c r="F5" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G5" s="29">
         <v>10</v>
@@ -9288,7 +7332,7 @@
         <v>100</v>
       </c>
       <c r="F6" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G6" s="29">
         <v>10</v>
@@ -9329,7 +7373,7 @@
         <v>100</v>
       </c>
       <c r="F7" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G7" s="29">
         <v>10</v>
@@ -9370,7 +7414,7 @@
         <v>100</v>
       </c>
       <c r="F8" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G8" s="29">
         <v>10</v>
@@ -9411,7 +7455,7 @@
         <v>100</v>
       </c>
       <c r="F9" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G9" s="29">
         <v>10</v>
@@ -9452,7 +7496,7 @@
         <v>100</v>
       </c>
       <c r="F10" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G10" s="29">
         <v>10</v>
@@ -9493,7 +7537,7 @@
         <v>100</v>
       </c>
       <c r="F11" s="29">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="G11" s="29">
         <v>10</v>
@@ -9528,20 +7572,20 @@
       <c r="F12" s="29"/>
       <c r="G12" s="29"/>
       <c r="H12" s="55" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="I12" s="56"/>
       <c r="J12" s="56"/>
       <c r="K12" s="56"/>
       <c r="L12" s="57"/>
       <c r="M12" s="55" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="N12" s="57"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.4">
@@ -9563,52 +7607,52 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B16" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="H16" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B17" s="29" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E17" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="F17" s="29" t="s">
         <v>320</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B19" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B20" s="29" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.4">
@@ -9619,7 +7663,7 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.4">
@@ -9640,26 +7684,26 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B26" s="36" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C26" s="45" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="36" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F26" s="55" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="G26" s="57"/>
       <c r="H26" s="36" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.4">
@@ -9667,18 +7711,18 @@
         <v>9</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="36" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="55" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="G27" s="57"/>
       <c r="H27" s="36" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.4">
@@ -9686,14 +7730,14 @@
         <v>1</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="36" t="s">
         <v>106</v>
       </c>
       <c r="F28" s="55" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="G28" s="57"/>
       <c r="H28" s="36">
@@ -9705,14 +7749,14 @@
         <v>2</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="36" t="s">
         <v>32</v>
       </c>
       <c r="F29" s="55" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="G29" s="57"/>
       <c r="H29" s="36">
@@ -9724,14 +7768,14 @@
         <v>3</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="36" t="s">
         <v>33</v>
       </c>
       <c r="F30" s="55" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="G30" s="57"/>
       <c r="H30" s="36">
@@ -9743,14 +7787,14 @@
         <v>4</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="36" t="s">
         <v>34</v>
       </c>
       <c r="F31" s="55" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="G31" s="57"/>
       <c r="H31" s="36">
@@ -9762,14 +7806,14 @@
         <v>5</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="36" t="s">
         <v>35</v>
       </c>
       <c r="F32" s="55" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="G32" s="57"/>
       <c r="H32" s="36">
@@ -9781,14 +7825,14 @@
         <v>6</v>
       </c>
       <c r="C33" s="45" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="36" t="s">
         <v>36</v>
       </c>
       <c r="F33" s="55" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G33" s="57"/>
       <c r="H33" s="36">
@@ -9800,14 +7844,14 @@
         <v>7</v>
       </c>
       <c r="C34" s="45" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="36" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="55" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G34" s="57"/>
       <c r="H34" s="36">
@@ -9819,14 +7863,14 @@
         <v>8</v>
       </c>
       <c r="C35" s="45" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="36" t="s">
         <v>38</v>
       </c>
       <c r="F35" s="55" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G35" s="57"/>
       <c r="H35" s="36">
@@ -9835,27 +7879,27 @@
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.4">
       <c r="H36" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B39" s="40" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="40" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F39" s="46" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="G39" s="46"/>
     </row>
@@ -9864,14 +7908,14 @@
         <v>9</v>
       </c>
       <c r="C40" s="45" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="40" t="s">
         <v>10</v>
       </c>
       <c r="F40" s="46" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="G40" s="46"/>
     </row>
@@ -9884,7 +7928,7 @@
       </c>
       <c r="D41" s="58"/>
       <c r="E41" s="40" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="F41" s="45">
         <v>1</v>
@@ -9900,7 +7944,7 @@
       </c>
       <c r="D42" s="58"/>
       <c r="E42" s="40" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="F42" s="45">
         <v>1</v>
@@ -9916,7 +7960,7 @@
       </c>
       <c r="D43" s="59"/>
       <c r="E43" s="40" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="F43" s="45">
         <v>2</v>
@@ -9932,7 +7976,7 @@
       </c>
       <c r="D44" s="58"/>
       <c r="E44" s="40" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="F44" s="45">
         <v>2</v>
@@ -9948,7 +7992,7 @@
       </c>
       <c r="D45" s="58"/>
       <c r="E45" s="40" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="F45" s="45">
         <v>2</v>
@@ -9964,7 +8008,7 @@
       </c>
       <c r="D46" s="58"/>
       <c r="E46" s="40" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="F46" s="45">
         <v>3</v>
@@ -9980,7 +8024,7 @@
       </c>
       <c r="D47" s="58"/>
       <c r="E47" s="40" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="F47" s="45">
         <v>3</v>
@@ -9996,7 +8040,7 @@
       </c>
       <c r="D48" s="58"/>
       <c r="E48" s="40" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="F48" s="45">
         <v>3</v>
@@ -10012,7 +8056,7 @@
       </c>
       <c r="D49" s="58"/>
       <c r="E49" s="40" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F49" s="45">
         <v>3</v>
@@ -10028,7 +8072,7 @@
       </c>
       <c r="D50" s="58"/>
       <c r="E50" s="40" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="F50" s="45">
         <v>3</v>
@@ -10037,29 +8081,29 @@
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.4">
       <c r="F51" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B53" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B54" s="35" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D54" s="33" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="F54" s="33" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.4">
@@ -10070,13 +8114,13 @@
         <v>9</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E55" s="33" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="F55" s="33" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.4">
@@ -10166,43 +8210,43 @@
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.4">
       <c r="C61" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D61" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E61" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="F61" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.4">
       <c r="B64" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="65" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B65" s="45" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C65" s="45"/>
       <c r="D65" s="45" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E65" s="45"/>
       <c r="F65" s="33" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="G65" s="33" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H65" s="33" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="I65" s="33" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.4">
@@ -10211,20 +8255,20 @@
       </c>
       <c r="C66" s="45"/>
       <c r="D66" s="45" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="E66" s="45"/>
       <c r="F66" s="33" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="G66" s="33" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="H66" s="33" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="I66" s="33" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.4">
@@ -10233,11 +8277,11 @@
       </c>
       <c r="C67" s="45"/>
       <c r="D67" s="45" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E67" s="45"/>
       <c r="F67" s="33" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="G67" s="33">
         <v>0</v>
@@ -10255,11 +8299,11 @@
       </c>
       <c r="C68" s="45"/>
       <c r="D68" s="45" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E68" s="45"/>
       <c r="F68" s="33" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="G68" s="33">
         <v>20</v>
@@ -10277,11 +8321,11 @@
       </c>
       <c r="C69" s="45"/>
       <c r="D69" s="45" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E69" s="45"/>
       <c r="F69" s="33" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="G69" s="33">
         <v>40</v>
@@ -10295,82 +8339,82 @@
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.4">
       <c r="G70" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="H70" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="I70" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B73" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="F73" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="J73" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B74" s="36" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="C74" s="36" t="s">
+        <v>423</v>
+      </c>
+      <c r="D74" s="36" t="s">
+        <v>424</v>
+      </c>
+      <c r="F74" s="36" t="s">
         <v>421</v>
       </c>
-      <c r="D74" s="36" t="s">
-        <v>422</v>
-      </c>
-      <c r="F74" s="36" t="s">
-        <v>419</v>
-      </c>
       <c r="G74" s="36" t="s">
+        <v>423</v>
+      </c>
+      <c r="H74" s="36" t="s">
+        <v>424</v>
+      </c>
+      <c r="J74" s="36" t="s">
         <v>421</v>
       </c>
-      <c r="H74" s="36" t="s">
-        <v>422</v>
-      </c>
-      <c r="J74" s="36" t="s">
-        <v>419</v>
-      </c>
       <c r="K74" s="36" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="L74" s="36" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="D75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="F75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="G75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="H75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="J75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="K75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="L75" s="36" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.4">
@@ -11825,22 +9869,22 @@
     </row>
     <row r="126" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C126" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D126" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="G126" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="H126" t="s">
+        <v>449</v>
+      </c>
+      <c r="K126" t="s">
         <v>447</v>
       </c>
-      <c r="K126" t="s">
-        <v>445</v>
-      </c>
       <c r="L126" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
   </sheetData>
@@ -11925,7 +9969,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
@@ -11935,7 +9979,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
@@ -11945,7 +9989,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
@@ -11955,17 +9999,17 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.4">

</xml_diff>